<commit_message>
Implementacion de la version 4 del reporte de facturacion
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
@@ -1,43 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">EfectorSigehos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EfectorSigehosExcel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EfectorObjetivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zubizarrete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santa Lucía</t>
+    <t>EfectorSigehos</t>
+  </si>
+  <si>
+    <t>EfectorSigehosExcel</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>EfectorObjetivos</t>
+  </si>
+  <si>
+    <t>Zubizarrete</t>
+  </si>
+  <si>
+    <t>Santa Lucía</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -66,13 +72,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -354,45 +372,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatizacion del Excel de CRG
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
@@ -1,49 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>EfectorSigehos</t>
+    <t xml:space="preserve">EfectorSigehos</t>
   </si>
   <si>
-    <t>EfectorSigehosExcel</t>
+    <t xml:space="preserve">EfectorSigehosExcel</t>
   </si>
   <si>
-    <t>ID</t>
+    <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t>EfectorObjetivos</t>
-  </si>
-  <si>
-    <t>Zubizarrete</t>
-  </si>
-  <si>
-    <t>Santa Lucía</t>
+    <t xml:space="preserve">EfectorObjetivos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -72,25 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -372,46 +348,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avances automatizacion reporte Sigehos
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">EfectorSigehos</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t xml:space="preserve">EfectorObjetivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOSP..DE.REHABILITACION.PSICOFISICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IREP</t>
   </si>
 </sst>
 </file>
@@ -369,6 +375,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Reporte SIGEHOS CRG Automatizado
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">EfectorSigehos</t>
   </si>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t xml:space="preserve">EfectorObjetivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOSP..DE.REHABILITACION.PSICOFISICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IREP</t>
   </si>
 </sst>
 </file>
@@ -375,18 +369,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Correccion de Fechas solapa CRG
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">EfectorSigehos</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t xml:space="preserve">EfectorObjetivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOSP..DE.REHABILITACION.PSICOFISICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IREP</t>
   </si>
 </sst>
 </file>
@@ -369,6 +375,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Resolucion Encoding de CRG y DPH, colocacion codigo duro por error de lectura y columna financiador bien nombrado
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Control-Sigehos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">EfectorSigehos</t>
   </si>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t xml:space="preserve">EfectorObjetivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOSP..DE.REHABILITACION.PSICOFISICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IREP</t>
   </si>
 </sst>
 </file>
@@ -375,18 +369,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>